<commit_message>
Update web content to display table views.
</commit_message>
<xml_diff>
--- a/assets/examples/xlsx/RS0002SimpleExampleFile.a205.xlsx
+++ b/assets/examples/xlsx/RS0002SimpleExampleFile.a205.xlsx
@@ -8,8 +8,8 @@
   </bookViews>
   <sheets>
     <sheet name="RS0002" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="performance_map_cooling" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="performance_map_standby" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="RS0004.performance_map_cooling" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="RS0004.performance_map_standby" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -136,14 +136,24 @@
         <t>Additional Information</t>
       </text>
     </comment>
+    <comment authorId="0" ref="A16" shapeId="0">
+      <text>
+        <t>Data group describing product information</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="B17" shapeId="0">
+      <text>
+        <t>Name of the manufacturer</t>
+      </text>
+    </comment>
     <comment authorId="0" ref="B18" shapeId="0">
       <text>
-        <t>Manufacturer name</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="B19" shapeId="0">
-      <text>
-        <t>Model number</t>
+        <t>Model number for this chiller</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="B20" shapeId="0">
+      <text>
+        <t>Continuous unit power draw regardless of whether the fan or DX system are operating.</t>
       </text>
     </comment>
     <comment authorId="0" ref="A22" shapeId="0">
@@ -201,47 +211,52 @@
         <t>Additional Information</t>
       </text>
     </comment>
+    <comment authorId="0" ref="A36" shapeId="0">
+      <text>
+        <t>Data group describing product information</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="B37" shapeId="0">
+      <text>
+        <t>Name of the outdoor unit manufacturer</t>
+      </text>
+    </comment>
     <comment authorId="0" ref="B38" shapeId="0">
       <text>
-        <t>Name of the outdoor unit manufacturer</t>
+        <t>Model number of the outdoor unit</t>
       </text>
     </comment>
     <comment authorId="0" ref="B39" shapeId="0">
       <text>
-        <t>Model number of the outdoor unit</t>
+        <t>Name of the indoor unit manufacturer</t>
       </text>
     </comment>
     <comment authorId="0" ref="B40" shapeId="0">
       <text>
-        <t>Name of the indoor unit manufacturer</t>
+        <t>Model number of the indoor unit</t>
       </text>
     </comment>
     <comment authorId="0" ref="B41" shapeId="0">
       <text>
-        <t>Model number of the indoor unit</t>
+        <t>Type of refrigerant</t>
       </text>
     </comment>
     <comment authorId="0" ref="B42" shapeId="0">
       <text>
-        <t>Type of refrigerant</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="B43" shapeId="0">
-      <text>
         <t>Type of compressor</t>
       </text>
     </comment>
-    <comment authorId="0" ref="B46" shapeId="0">
-      <text>
-        <t>Cycling degradation coefficient (CD) as described in AHRI 210/240</t>
+    <comment authorId="0" ref="B45" shapeId="0">
+      <text>
+        <t>Cycling degradation coefficient (CD) as described in AHRI 550/590 or AHRI 551/591</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="A46" shapeId="0">
+      <text>
+        <t>Data group describing cooling performance over a range of conditions</t>
       </text>
     </comment>
     <comment authorId="0" ref="A47" shapeId="0">
-      <text>
-        <t>Data group describing cooling performance over a range of conditions</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="A48" shapeId="0">
       <text>
         <t>Data group describing standby performance</t>
       </text>
@@ -328,7 +343,7 @@
     </comment>
     <comment authorId="0" ref="B2" shapeId="0">
       <text>
-        <t>Data group defining the grid variables for standby performance</t>
+        <t>Data group defining the lookup variables for standby performance</t>
       </text>
     </comment>
     <comment authorId="0" ref="A3" shapeId="0">
@@ -634,7 +649,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -863,7 +878,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>ASHRAE205.RS_instance.RS0002</t>
+          <t>ASHRAE205.RS_instance.description</t>
         </is>
       </c>
       <c r="E15" s="3" t="n"/>
@@ -871,28 +886,37 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>ASHRAE205.RS_instance.RS0002.description</t>
+          <t>ASHRAE205.RS_instance.description.product_information</t>
         </is>
       </c>
       <c r="E16" s="3" t="n"/>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>ASHRAE205.RS_instance.RS0002.description.product_information</t>
-        </is>
-      </c>
-      <c r="E17" s="3" t="n"/>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">            manufacturer</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>ColdAirInc</t>
+        </is>
+      </c>
+      <c r="E17" s="3" t="inlineStr">
+        <is>
+          <t>✓</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="B18" t="inlineStr">
         <is>
-          <t xml:space="preserve">                manufacturer</t>
+          <t xml:space="preserve">            model_number</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>ColdAirInc</t>
+          <t>AC.2019.01</t>
         </is>
       </c>
       <c r="E18" s="3" t="inlineStr">
@@ -902,38 +926,33 @@
       </c>
     </row>
     <row r="19">
-      <c r="B19" t="inlineStr">
-        <is>
-          <t xml:space="preserve">                model_number</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>AC.2019.01</t>
-        </is>
-      </c>
-      <c r="E19" s="3" t="inlineStr">
-        <is>
-          <t>✓</t>
-        </is>
-      </c>
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>ASHRAE205.RS_instance.performance</t>
+        </is>
+      </c>
+      <c r="E19" s="3" t="n"/>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>ASHRAE205.RS_instance.RS0002.performance</t>
-        </is>
-      </c>
-      <c r="E20" s="3" t="inlineStr">
-        <is>
-          <t>✓</t>
-        </is>
-      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">        standby_power</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>999</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
+      <c r="E20" s="3" t="n"/>
     </row>
     <row r="21">
       <c r="B21" t="inlineStr">
         <is>
-          <t xml:space="preserve">            fan_position</t>
+          <t xml:space="preserve">        fan_position</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -941,28 +960,20 @@
           <t>BLOW_THROUGH</t>
         </is>
       </c>
-      <c r="E21" s="3" t="inlineStr">
-        <is>
-          <t>✓</t>
-        </is>
-      </c>
+      <c r="E21" s="3" t="n"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>ASHRAE205.RS_instance.RS0002.performance.coil_system_representation</t>
-        </is>
-      </c>
-      <c r="E22" s="3" t="inlineStr">
-        <is>
-          <t>✓</t>
-        </is>
-      </c>
+          <t>ASHRAE205.RS_instance.performance.DX_system_representation</t>
+        </is>
+      </c>
+      <c r="E22" s="3" t="n"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>ASHRAE205.RS_instance.RS0002.performance.coil_system_representation.ASHRAE205</t>
+          <t>ASHRAE205.RS_instance.performance.DX_system_representation.ASHRAE205</t>
         </is>
       </c>
       <c r="E23" s="3" t="n"/>
@@ -970,7 +981,7 @@
     <row r="24">
       <c r="B24" t="inlineStr">
         <is>
-          <t xml:space="preserve">                    standard_version</t>
+          <t xml:space="preserve">                standard_version</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -987,7 +998,7 @@
     <row r="25">
       <c r="B25" t="inlineStr">
         <is>
-          <t xml:space="preserve">                    schema_version</t>
+          <t xml:space="preserve">                schema_version</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1004,7 +1015,7 @@
     <row r="26">
       <c r="B26" t="inlineStr">
         <is>
-          <t xml:space="preserve">                    RS_ID</t>
+          <t xml:space="preserve">                RS_ID</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1021,7 +1032,7 @@
     <row r="27">
       <c r="B27" t="inlineStr">
         <is>
-          <t xml:space="preserve">                    description</t>
+          <t xml:space="preserve">                description</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1038,7 +1049,7 @@
     <row r="28">
       <c r="B28" t="inlineStr">
         <is>
-          <t xml:space="preserve">                    ID</t>
+          <t xml:space="preserve">                ID</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1055,7 +1066,7 @@
     <row r="29">
       <c r="B29" t="inlineStr">
         <is>
-          <t xml:space="preserve">                    data_timestamp</t>
+          <t xml:space="preserve">                data_timestamp</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1072,7 +1083,7 @@
     <row r="30">
       <c r="B30" t="inlineStr">
         <is>
-          <t xml:space="preserve">                    data_version</t>
+          <t xml:space="preserve">                data_version</t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -1087,7 +1098,7 @@
     <row r="31">
       <c r="B31" t="inlineStr">
         <is>
-          <t xml:space="preserve">                    data_source</t>
+          <t xml:space="preserve">                data_source</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1100,7 +1111,7 @@
     <row r="32">
       <c r="B32" t="inlineStr">
         <is>
-          <t xml:space="preserve">                    disclaimer</t>
+          <t xml:space="preserve">                disclaimer</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1113,7 +1124,7 @@
     <row r="33">
       <c r="B33" t="inlineStr">
         <is>
-          <t xml:space="preserve">                    notes</t>
+          <t xml:space="preserve">                notes</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1126,7 +1137,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>ASHRAE205.RS_instance.RS0002.performance.coil_system_representation.ASHRAE205.RS_instance</t>
+          <t>ASHRAE205.RS_instance.performance.DX_system_representation.ASHRAE205.RS_instance</t>
         </is>
       </c>
       <c r="E34" s="3" t="inlineStr">
@@ -1138,7 +1149,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>ASHRAE205.RS_instance.RS0002.performance.coil_system_representation.ASHRAE205.RS_instance.RS0004</t>
+          <t>ASHRAE205.RS_instance.performance.DX_system_representation.ASHRAE205.RS_instance.description</t>
         </is>
       </c>
       <c r="E35" s="3" t="n"/>
@@ -1146,15 +1157,20 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>ASHRAE205.RS_instance.RS0002.performance.coil_system_representation.ASHRAE205.RS_instance.RS0004.description</t>
+          <t>ASHRAE205.RS_instance.performance.DX_system_representation.ASHRAE205.RS_instance.description.product_information</t>
         </is>
       </c>
       <c r="E36" s="3" t="n"/>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>ASHRAE205.RS_instance.RS0002.performance.coil_system_representation.ASHRAE205.RS_instance.RS0004.description.product_information</t>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">                            outdoor_unit_manufacturer</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>ColdAirInc</t>
         </is>
       </c>
       <c r="E37" s="3" t="n"/>
@@ -1162,46 +1178,38 @@
     <row r="38">
       <c r="B38" t="inlineStr">
         <is>
-          <t xml:space="preserve">                                    outdoor_unit_manufacturer</t>
+          <t xml:space="preserve">                            outdoor_unit_model_number</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>ColdAirInc</t>
-        </is>
-      </c>
-      <c r="E38" s="3" t="inlineStr">
-        <is>
-          <t>✓</t>
-        </is>
-      </c>
+          <t>AC.2019.01</t>
+        </is>
+      </c>
+      <c r="E38" s="3" t="n"/>
     </row>
     <row r="39">
       <c r="B39" t="inlineStr">
         <is>
-          <t xml:space="preserve">                                    outdoor_unit_model_number</t>
+          <t xml:space="preserve">                            indoor_unit_manufacturer</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>AC.2019.01</t>
-        </is>
-      </c>
-      <c r="E39" s="3" t="inlineStr">
-        <is>
-          <t>✓</t>
-        </is>
-      </c>
+          <t>ColdAirInc</t>
+        </is>
+      </c>
+      <c r="E39" s="3" t="n"/>
     </row>
     <row r="40">
       <c r="B40" t="inlineStr">
         <is>
-          <t xml:space="preserve">                                    indoor_unit_manufacturer</t>
+          <t xml:space="preserve">                            indoor_unit_model_number</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>ColdAirInc</t>
+          <t>AC.2019.02</t>
         </is>
       </c>
       <c r="E40" s="3" t="n"/>
@@ -1209,12 +1217,12 @@
     <row r="41">
       <c r="B41" t="inlineStr">
         <is>
-          <t xml:space="preserve">                                    indoor_unit_model_number</t>
+          <t xml:space="preserve">                            refrigerant_type</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>AC.2019.02</t>
+          <t>R410A</t>
         </is>
       </c>
       <c r="E41" s="3" t="n"/>
@@ -1222,66 +1230,63 @@
     <row r="42">
       <c r="B42" t="inlineStr">
         <is>
-          <t xml:space="preserve">                                    refrigerant_type</t>
+          <t xml:space="preserve">                            compressor_type</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>R410A</t>
+          <t>SCROLL</t>
         </is>
       </c>
       <c r="E42" s="3" t="n"/>
     </row>
     <row r="43">
-      <c r="B43" t="inlineStr">
-        <is>
-          <t xml:space="preserve">                                    compressor_type</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>SCROLL</t>
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>ASHRAE205.RS_instance.performance.DX_system_representation.ASHRAE205.RS_instance.performance</t>
         </is>
       </c>
       <c r="E43" s="3" t="n"/>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>ASHRAE205.RS_instance.RS0002.performance.coil_system_representation.ASHRAE205.RS_instance.RS0004.performance</t>
-        </is>
-      </c>
-      <c r="E44" s="3" t="inlineStr">
-        <is>
-          <t>✓</t>
-        </is>
-      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t xml:space="preserve">                        compressor_control_method</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>DYNAMIC</t>
+        </is>
+      </c>
+      <c r="E44" s="3" t="n"/>
     </row>
     <row r="45">
       <c r="B45" t="inlineStr">
         <is>
-          <t xml:space="preserve">                                compressor_control_method</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>DYNAMIC</t>
-        </is>
-      </c>
-      <c r="E45" s="3" t="inlineStr">
-        <is>
-          <t>✓</t>
-        </is>
-      </c>
+          <t xml:space="preserve">                        cycling_degradation_coefficient</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E45" s="3" t="n"/>
     </row>
     <row r="46">
-      <c r="B46" t="inlineStr">
-        <is>
-          <t xml:space="preserve">                                cycling_degradation_coefficient</t>
-        </is>
-      </c>
-      <c r="C46" t="n">
-        <v>0.25</v>
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>ASHRAE205.RS_instance.performance.DX_system_representation.ASHRAE205.RS_instance.performance.performance_map_cooling</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>$RS0004.performance_map_cooling</t>
+        </is>
       </c>
       <c r="E46" s="3" t="inlineStr">
         <is>
@@ -1292,32 +1297,15 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>ASHRAE205.RS_instance.RS0002.performance.coil_system_representation.ASHRAE205.RS_instance.RS0004.performance.performance_map_cooling</t>
+          <t>ASHRAE205.RS_instance.performance.DX_system_representation.ASHRAE205.RS_instance.performance.performance_map_standby</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>$performance_map_cooling</t>
+          <t>$RS0004.performance_map_standby</t>
         </is>
       </c>
       <c r="E47" s="3" t="inlineStr">
-        <is>
-          <t>✓</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>ASHRAE205.RS_instance.RS0002.performance.coil_system_representation.ASHRAE205.RS_instance.RS0004.performance.performance_map_standby</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>$performance_map_standby</t>
-        </is>
-      </c>
-      <c r="E48" s="3" t="inlineStr">
         <is>
           <t>✓</t>
         </is>
@@ -1329,7 +1317,7 @@
       <formula1>"PPR2"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C6" type="list">
-      <formula1>"RS0001,RS0002,RS0003,RS0004"</formula1>
+      <formula1>"RS0001,RS0002,RS0003,RS0004,RS0005,RS0006"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C21" type="list">
       <formula1>"BLOW_THROUGH,DRAW_THROUGH"</formula1>
@@ -1338,12 +1326,12 @@
       <formula1>"PPR2"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C26" type="list">
-      <formula1>"RS0001,RS0002,RS0003,RS0004"</formula1>
+      <formula1>"RS0001,RS0002,RS0003,RS0004,RS0005,RS0006"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C43" type="list">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C42" type="list">
       <formula1>"RECIPROCATING,SCREW,CENTRIFUGAL,ROTARY,SCROLL"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C45" type="list">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C44" type="list">
       <formula1>"STAGED,DYNAMIC"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1369,7 +1357,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>ASHRAE205.RS_instance.RS0002.performance.coil_system_representation.ASHRAE205.RS_instance.RS0004.performance.performance_map_cooling.grid_variables</t>
+          <t>ASHRAE205.RS_instance.performance.DX_system_representation.ASHRAE205.RS_instance.performance.performance_map_cooling.grid_variables</t>
         </is>
       </c>
     </row>
@@ -2542,7 +2530,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>ASHRAE205.RS_instance.RS0002.performance.coil_system_representation.ASHRAE205.RS_instance.RS0004.performance.performance_map_standby.grid_variables</t>
+          <t>ASHRAE205.RS_instance.performance.DX_system_representation.ASHRAE205.RS_instance.performance.performance_map_standby.grid_variables</t>
         </is>
       </c>
     </row>

</xml_diff>